<commit_message>
It is now showing a map for one pair of places, length of miile and with of span set by variables that can be changed.
</commit_message>
<xml_diff>
--- a/SchnitlerBasis.xlsx
+++ b/SchnitlerBasis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oeide/sciebo/koln/forskning/Space/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oeide/Documents/GitHub/space-exploration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7145C676-7462-F647-84CD-77FE53BB26CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB99A14-6B11-C842-89D4-99C6CA3A8C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2760" yWindow="5400" windowWidth="27840" windowHeight="16740" xr2:uid="{4BD8D586-FF64-C244-8902-BC705B4844D2}"/>
   </bookViews>
@@ -605,7 +605,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>